<commit_message>
Parameter sets for the 8 videos produced by nbody.py
</commit_message>
<xml_diff>
--- a/Source-Code/nbody_parameter_sets.xlsx
+++ b/Source-Code/nbody_parameter_sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFD50B11-8418-4121-9B96-1C0A01A8D23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D724C4-42AB-48DA-A2D5-FFA77B6B33C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="13030" windowHeight="9430" xr2:uid="{B660C301-AE00-487A-9B15-DC0AB9180F8F}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="16790" windowHeight="9430" xr2:uid="{B660C301-AE00-487A-9B15-DC0AB9180F8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
   <si>
     <t>params</t>
   </si>
@@ -150,16 +150,43 @@
   </si>
   <si>
     <t>my_dpi</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Nstars</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Set 8</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -193,6 +220,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,20 +535,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8F3FDD-E818-47F6-829F-7515B87F404D}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -543,8 +574,11 @@
       <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -569,8 +603,11 @@
       <c r="H3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -595,8 +632,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -621,8 +661,11 @@
       <c r="H5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -647,8 +690,11 @@
       <c r="H6">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -673,8 +719,11 @@
       <c r="H7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -699,8 +748,11 @@
       <c r="H8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -725,8 +777,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -751,34 +806,40 @@
       <c r="H10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>0.2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>0.2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>0.2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>0.8</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>0.8</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>0.8</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -803,8 +864,11 @@
       <c r="H12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -829,8 +893,11 @@
       <c r="H13">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -855,8 +922,11 @@
       <c r="H14" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -881,8 +951,11 @@
       <c r="H15" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -907,8 +980,11 @@
       <c r="H16" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -933,8 +1009,11 @@
       <c r="H17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -959,8 +1038,11 @@
       <c r="H18" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -985,8 +1067,11 @@
       <c r="H19" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1011,63 +1096,131 @@
       <c r="H20" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
-      <c r="E21">
-        <v>20</v>
-      </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-      <c r="G21">
-        <v>20</v>
-      </c>
-      <c r="H21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>20</v>
+      </c>
+      <c r="I23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>240</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>240</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>240</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>240</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>240</v>
       </c>
-      <c r="G22">
+      <c r="G24">
         <v>240</v>
       </c>
-      <c r="H22">
+      <c r="H24">
         <v>240</v>
       </c>
+      <c r="I24">
+        <v>240</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B17:H18" numberStoredAsText="1"/>
+    <ignoredError sqref="B17:H18 B21:H22 I21:I22 I17:I18" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>